<commit_message>
Project StudioIssues.TestGitUsersWorkSimultaneously is saved. Author: user131. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/StudioIssues.TestGitUsersWorkSimultaneously/Bank Rating.xlsx
+++ b/DESIGN/rules/StudioIssues.TestGitUsersWorkSimultaneously/Bank Rating.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="699">
   <si>
     <t>&gt; 51</t>
   </si>
@@ -4084,6 +4084,9 @@
       </rPr>
       <t xml:space="preserve"> (Bank bank, RatingGroup bankRatingGroup)</t>
     </r>
+  </si>
+  <si>
+    <t>R5,R4,R3,R2,R1</t>
   </si>
 </sst>
 </file>
@@ -4182,7 +4185,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="0" rgb="FFFFFF"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
     </font>
@@ -4217,7 +4220,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="2" tint="-0.749992370372631"/>
+      <color theme="2" tint="-0.749992370372631" rgb="EEECE1"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
       <charset val="204"/>
@@ -4294,7 +4297,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="-0.249977111117893" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4306,13 +4309,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="0.39997558519241921" rgb="9BBB59"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4330,13 +4333,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2" rgb="EEECE1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5083,13 +5086,13 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -5153,40 +5156,40 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -5367,7 +5370,7 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top/>
       <bottom/>
@@ -5403,14 +5406,14 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5421,7 +5424,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5447,7 +5450,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5458,7 +5461,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5471,22 +5474,22 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5731,58 +5734,58 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
+        <color theme="0" tint="-0.249977111117893" rgb="FFFFFF"/>
       </right>
       <top/>
       <bottom/>
@@ -6381,13 +6384,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="3"/>
   </cellStyleXfs>
   <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -6410,13 +6411,13 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -6492,7 +6493,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="5"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="3"/>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6505,14 +6506,14 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="64" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="5" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6753,7 +6754,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="146" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="147" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="147" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="148" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="149" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="124" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7114,13 +7115,11 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Heading 1" xfId="5" builtinId="16"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 7" xfId="3"/>
     <cellStyle name="Normal_EPLI rater" xfId="1"/>
-    <cellStyle name="Обычный 2" xfId="2"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -7513,17 +7512,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5" collapsed="1"/>
-    <col min="2" max="2" width="9.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="76.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="5.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="25" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" style="5" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="8.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="25.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="42.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="5" width="76.7109375" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="5" width="5.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="25.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="5" width="19.140625" collapsed="true"/>
+    <col min="12" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
@@ -8533,9 +8532,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -8718,9 +8717,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -8849,8 +8848,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -8955,18 +8954,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="44.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="4.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="3.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -9147,7 +9146,9 @@
       <c r="E14" s="23" t="s">
         <v>329</v>
       </c>
-      <c r="F14" s="229"/>
+      <c r="F14" s="229" t="s">
+        <v>698</v>
+      </c>
       <c r="G14" s="257">
         <v>1</v>
       </c>
@@ -9478,9 +9479,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -9565,9 +9566,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2" collapsed="1"/>
-    <col min="3" max="3" width="35.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="2" style="2" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="35.85546875" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
@@ -9635,10 +9636,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="48.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="48.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
@@ -9931,8 +9932,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -10016,10 +10017,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="39.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="2" style="2" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="39.140625" collapsed="true"/>
+    <col min="5" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -10443,10 +10444,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="2" collapsed="1"/>
-    <col min="4" max="4" width="34.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="3" style="2" width="9.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="34.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="30.0" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -10843,9 +10844,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -11115,27 +11116,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="51.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="48.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="29.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10" style="2" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="25" style="2" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="21" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="3.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="21.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="28.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="51.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="30.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="32.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="48.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="29.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="10.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="2" width="21.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="25.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="38.7109375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="2" width="23.140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="2" width="19.42578125" collapsed="true"/>
+    <col min="21" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -12347,10 +12348,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4" collapsed="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="4" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -13069,10 +13070,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -13167,9 +13168,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="30" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -13473,9 +13474,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -13579,8 +13580,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="4" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -13946,9 +13947,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -14113,12 +14114,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="15" collapsed="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="15" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="44.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="40.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>